<commit_message>
replace flooding data from matt
</commit_message>
<xml_diff>
--- a/data-raw/CLIMATE_BG20.xlsx
+++ b/data-raw/CLIMATE_BG20.xlsx
@@ -9461,8 +9461,12 @@
       <c r="C37" t="n">
         <v>0.06</v>
       </c>
-      <c r="D37"/>
-      <c r="E37"/>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
       <c r="F37" t="n">
         <v>8.21</v>
       </c>
@@ -9571,8 +9575,12 @@
       <c r="C40" t="n">
         <v>0.094</v>
       </c>
-      <c r="D40"/>
-      <c r="E40"/>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
       <c r="F40" t="n">
         <v>6.69</v>
       </c>
@@ -9757,8 +9765,12 @@
       <c r="C45" t="n">
         <v>0.089</v>
       </c>
-      <c r="D45"/>
-      <c r="E45"/>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
       <c r="F45" t="n">
         <v>15.95</v>
       </c>
@@ -9791,8 +9803,12 @@
       <c r="C46" t="n">
         <v>0.086</v>
       </c>
-      <c r="D46"/>
-      <c r="E46"/>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
       <c r="F46" t="n">
         <v>6.19</v>
       </c>
@@ -10015,8 +10031,12 @@
       <c r="C52" t="n">
         <v>0.118</v>
       </c>
-      <c r="D52"/>
-      <c r="E52"/>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
       <c r="F52" t="n">
         <v>7.32</v>
       </c>
@@ -10125,8 +10145,12 @@
       <c r="C55" t="n">
         <v>0.116</v>
       </c>
-      <c r="D55"/>
-      <c r="E55"/>
+      <c r="D55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
       <c r="F55" t="n">
         <v>7.85</v>
       </c>
@@ -10159,8 +10183,12 @@
       <c r="C56" t="n">
         <v>0.067</v>
       </c>
-      <c r="D56"/>
-      <c r="E56"/>
+      <c r="D56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
       <c r="F56" t="n">
         <v>8.05</v>
       </c>
@@ -10307,8 +10335,12 @@
       <c r="C60" t="n">
         <v>0.11</v>
       </c>
-      <c r="D60"/>
-      <c r="E60"/>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0</v>
+      </c>
       <c r="F60" t="n">
         <v>8.13</v>
       </c>
@@ -10607,8 +10639,12 @@
       <c r="C68" t="n">
         <v>0.069</v>
       </c>
-      <c r="D68"/>
-      <c r="E68"/>
+      <c r="D68" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0</v>
+      </c>
       <c r="F68" t="n">
         <v>10.89</v>
       </c>
@@ -10679,8 +10715,12 @@
       <c r="C70" t="n">
         <v>0.095</v>
       </c>
-      <c r="D70"/>
-      <c r="E70"/>
+      <c r="D70" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0</v>
+      </c>
       <c r="F70"/>
       <c r="G70"/>
       <c r="H70"/>
@@ -10837,8 +10877,12 @@
       <c r="C75" t="n">
         <v>0.103</v>
       </c>
-      <c r="D75"/>
-      <c r="E75"/>
+      <c r="D75" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0</v>
+      </c>
       <c r="F75" t="n">
         <v>7.31</v>
       </c>
@@ -11403,8 +11447,12 @@
       <c r="C90" t="n">
         <v>0.174</v>
       </c>
-      <c r="D90"/>
-      <c r="E90"/>
+      <c r="D90" t="n">
+        <v>0</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0</v>
+      </c>
       <c r="F90" t="n">
         <v>7.58</v>
       </c>
@@ -11475,8 +11523,12 @@
       <c r="C92" t="n">
         <v>0.041</v>
       </c>
-      <c r="D92"/>
-      <c r="E92"/>
+      <c r="D92" t="n">
+        <v>0</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0</v>
+      </c>
       <c r="F92" t="n">
         <v>6.21</v>
       </c>
@@ -11585,8 +11637,12 @@
       <c r="C95" t="n">
         <v>0.097</v>
       </c>
-      <c r="D95"/>
-      <c r="E95"/>
+      <c r="D95" t="n">
+        <v>0</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0</v>
+      </c>
       <c r="F95" t="n">
         <v>11.59</v>
       </c>
@@ -11771,8 +11827,12 @@
       <c r="C100" t="n">
         <v>0.118</v>
       </c>
-      <c r="D100"/>
-      <c r="E100"/>
+      <c r="D100" t="n">
+        <v>0</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0</v>
+      </c>
       <c r="F100" t="n">
         <v>7.81</v>
       </c>
@@ -11843,8 +11903,12 @@
       <c r="C102" t="n">
         <v>0.097</v>
       </c>
-      <c r="D102"/>
-      <c r="E102"/>
+      <c r="D102" t="n">
+        <v>0</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0</v>
+      </c>
       <c r="F102" t="n">
         <v>9.01</v>
       </c>
@@ -12205,8 +12269,12 @@
       <c r="C112" t="n">
         <v>0.092</v>
       </c>
-      <c r="D112"/>
-      <c r="E112"/>
+      <c r="D112" t="n">
+        <v>0</v>
+      </c>
+      <c r="E112" t="n">
+        <v>0</v>
+      </c>
       <c r="F112" t="n">
         <v>6.27</v>
       </c>
@@ -13037,8 +13105,12 @@
       <c r="C134" t="n">
         <v>0.081</v>
       </c>
-      <c r="D134"/>
-      <c r="E134"/>
+      <c r="D134" t="n">
+        <v>0</v>
+      </c>
+      <c r="E134" t="n">
+        <v>0</v>
+      </c>
       <c r="F134" t="n">
         <v>6.94</v>
       </c>
@@ -13071,8 +13143,12 @@
       <c r="C135" t="n">
         <v>0.089</v>
       </c>
-      <c r="D135"/>
-      <c r="E135"/>
+      <c r="D135" t="n">
+        <v>0</v>
+      </c>
+      <c r="E135" t="n">
+        <v>0</v>
+      </c>
       <c r="F135" t="n">
         <v>7.63</v>
       </c>
@@ -13395,8 +13471,12 @@
       <c r="C144" t="n">
         <v>0.071</v>
       </c>
-      <c r="D144"/>
-      <c r="E144"/>
+      <c r="D144" t="n">
+        <v>0</v>
+      </c>
+      <c r="E144" t="n">
+        <v>0</v>
+      </c>
       <c r="F144" t="n">
         <v>7.08</v>
       </c>
@@ -13923,8 +14003,12 @@
       <c r="C158" t="n">
         <v>0.053</v>
       </c>
-      <c r="D158"/>
-      <c r="E158"/>
+      <c r="D158" t="n">
+        <v>0</v>
+      </c>
+      <c r="E158" t="n">
+        <v>0</v>
+      </c>
       <c r="F158" t="n">
         <v>7.26</v>
       </c>
@@ -13995,8 +14079,12 @@
       <c r="C160" t="n">
         <v>0.072</v>
       </c>
-      <c r="D160"/>
-      <c r="E160"/>
+      <c r="D160" t="n">
+        <v>0</v>
+      </c>
+      <c r="E160" t="n">
+        <v>0</v>
+      </c>
       <c r="F160" t="n">
         <v>7.5</v>
       </c>
@@ -14029,8 +14117,12 @@
       <c r="C161" t="n">
         <v>0.075</v>
       </c>
-      <c r="D161"/>
-      <c r="E161"/>
+      <c r="D161" t="n">
+        <v>0</v>
+      </c>
+      <c r="E161" t="n">
+        <v>0</v>
+      </c>
       <c r="F161" t="n">
         <v>6.57</v>
       </c>
@@ -14329,8 +14421,12 @@
       <c r="C169" t="n">
         <v>0.078</v>
       </c>
-      <c r="D169"/>
-      <c r="E169"/>
+      <c r="D169" t="n">
+        <v>0</v>
+      </c>
+      <c r="E169" t="n">
+        <v>0</v>
+      </c>
       <c r="F169" t="n">
         <v>7.47</v>
       </c>
@@ -14401,8 +14497,12 @@
       <c r="C171" t="n">
         <v>0.084</v>
       </c>
-      <c r="D171"/>
-      <c r="E171"/>
+      <c r="D171" t="n">
+        <v>0</v>
+      </c>
+      <c r="E171" t="n">
+        <v>0</v>
+      </c>
       <c r="F171" t="n">
         <v>10.81</v>
       </c>
@@ -14625,8 +14725,12 @@
       <c r="C177" t="n">
         <v>0.145</v>
       </c>
-      <c r="D177"/>
-      <c r="E177"/>
+      <c r="D177" t="n">
+        <v>0</v>
+      </c>
+      <c r="E177" t="n">
+        <v>0</v>
+      </c>
       <c r="F177"/>
       <c r="G177"/>
       <c r="H177"/>
@@ -14645,8 +14749,12 @@
       <c r="C178" t="n">
         <v>0.038</v>
       </c>
-      <c r="D178"/>
-      <c r="E178"/>
+      <c r="D178" t="n">
+        <v>0</v>
+      </c>
+      <c r="E178" t="n">
+        <v>0</v>
+      </c>
       <c r="F178" t="n">
         <v>9.39</v>
       </c>
@@ -14931,8 +15039,12 @@
       <c r="C186" t="n">
         <v>0.088</v>
       </c>
-      <c r="D186"/>
-      <c r="E186"/>
+      <c r="D186" t="n">
+        <v>0</v>
+      </c>
+      <c r="E186" t="n">
+        <v>0</v>
+      </c>
       <c r="F186" t="n">
         <v>4.62</v>
       </c>
@@ -15231,8 +15343,12 @@
       <c r="C194" t="n">
         <v>0.099</v>
       </c>
-      <c r="D194"/>
-      <c r="E194"/>
+      <c r="D194" t="n">
+        <v>0</v>
+      </c>
+      <c r="E194" t="n">
+        <v>0</v>
+      </c>
       <c r="F194" t="n">
         <v>3.66</v>
       </c>
@@ -15265,8 +15381,12 @@
       <c r="C195" t="n">
         <v>0.104</v>
       </c>
-      <c r="D195"/>
-      <c r="E195"/>
+      <c r="D195" t="n">
+        <v>0</v>
+      </c>
+      <c r="E195" t="n">
+        <v>0</v>
+      </c>
       <c r="F195" t="n">
         <v>5.26</v>
       </c>
@@ -15337,8 +15457,12 @@
       <c r="C197" t="n">
         <v>0.209</v>
       </c>
-      <c r="D197"/>
-      <c r="E197"/>
+      <c r="D197" t="n">
+        <v>0</v>
+      </c>
+      <c r="E197" t="n">
+        <v>0</v>
+      </c>
       <c r="F197" t="n">
         <v>6.67</v>
       </c>
@@ -15409,8 +15533,12 @@
       <c r="C199" t="n">
         <v>0.155</v>
       </c>
-      <c r="D199"/>
-      <c r="E199"/>
+      <c r="D199" t="n">
+        <v>0</v>
+      </c>
+      <c r="E199" t="n">
+        <v>0</v>
+      </c>
       <c r="F199" t="n">
         <v>3.6</v>
       </c>
@@ -15443,8 +15571,12 @@
       <c r="C200" t="n">
         <v>0.13</v>
       </c>
-      <c r="D200"/>
-      <c r="E200"/>
+      <c r="D200" t="n">
+        <v>0</v>
+      </c>
+      <c r="E200" t="n">
+        <v>0</v>
+      </c>
       <c r="F200" t="n">
         <v>6.68</v>
       </c>
@@ -15553,8 +15685,12 @@
       <c r="C203" t="n">
         <v>0.226</v>
       </c>
-      <c r="D203"/>
-      <c r="E203"/>
+      <c r="D203" t="n">
+        <v>0</v>
+      </c>
+      <c r="E203" t="n">
+        <v>0</v>
+      </c>
       <c r="F203" t="n">
         <v>13.04</v>
       </c>
@@ -15587,8 +15723,12 @@
       <c r="C204" t="n">
         <v>0.185</v>
       </c>
-      <c r="D204"/>
-      <c r="E204"/>
+      <c r="D204" t="n">
+        <v>0</v>
+      </c>
+      <c r="E204" t="n">
+        <v>0</v>
+      </c>
       <c r="F204" t="n">
         <v>9.81</v>
       </c>
@@ -15811,8 +15951,12 @@
       <c r="C210" t="n">
         <v>0.063</v>
       </c>
-      <c r="D210"/>
-      <c r="E210"/>
+      <c r="D210" t="n">
+        <v>0</v>
+      </c>
+      <c r="E210" t="n">
+        <v>0</v>
+      </c>
       <c r="F210" t="n">
         <v>8.53</v>
       </c>
@@ -16073,8 +16217,12 @@
       <c r="C217" t="n">
         <v>0.092</v>
       </c>
-      <c r="D217"/>
-      <c r="E217"/>
+      <c r="D217" t="n">
+        <v>0</v>
+      </c>
+      <c r="E217" t="n">
+        <v>0</v>
+      </c>
       <c r="F217"/>
       <c r="G217"/>
       <c r="H217"/>
@@ -16169,8 +16317,12 @@
       <c r="C220" t="n">
         <v>0.117</v>
       </c>
-      <c r="D220"/>
-      <c r="E220"/>
+      <c r="D220" t="n">
+        <v>0</v>
+      </c>
+      <c r="E220" t="n">
+        <v>0</v>
+      </c>
       <c r="F220" t="n">
         <v>6.82</v>
       </c>
@@ -18317,8 +18469,12 @@
       <c r="C277" t="n">
         <v>0.047</v>
       </c>
-      <c r="D277"/>
-      <c r="E277"/>
+      <c r="D277" t="n">
+        <v>0</v>
+      </c>
+      <c r="E277" t="n">
+        <v>0</v>
+      </c>
       <c r="F277" t="n">
         <v>8.42</v>
       </c>
@@ -18427,8 +18583,12 @@
       <c r="C280" t="n">
         <v>0.073</v>
       </c>
-      <c r="D280"/>
-      <c r="E280"/>
+      <c r="D280" t="n">
+        <v>0</v>
+      </c>
+      <c r="E280" t="n">
+        <v>0</v>
+      </c>
       <c r="F280" t="n">
         <v>10.76</v>
       </c>
@@ -19145,8 +19305,12 @@
       <c r="C299" t="n">
         <v>0.068</v>
       </c>
-      <c r="D299"/>
-      <c r="E299"/>
+      <c r="D299" t="n">
+        <v>0</v>
+      </c>
+      <c r="E299" t="n">
+        <v>0</v>
+      </c>
       <c r="F299" t="n">
         <v>11.55</v>
       </c>
@@ -19483,8 +19647,12 @@
       <c r="C308" t="n">
         <v>0.039</v>
       </c>
-      <c r="D308"/>
-      <c r="E308"/>
+      <c r="D308" t="n">
+        <v>0</v>
+      </c>
+      <c r="E308" t="n">
+        <v>0</v>
+      </c>
       <c r="F308" t="n">
         <v>6.6</v>
       </c>
@@ -19897,8 +20065,12 @@
       <c r="C319" t="n">
         <v>0.019</v>
       </c>
-      <c r="D319"/>
-      <c r="E319"/>
+      <c r="D319" t="n">
+        <v>0</v>
+      </c>
+      <c r="E319" t="n">
+        <v>0</v>
+      </c>
       <c r="F319" t="n">
         <v>12.67</v>
       </c>
@@ -19931,8 +20103,12 @@
       <c r="C320" t="n">
         <v>0.054</v>
       </c>
-      <c r="D320"/>
-      <c r="E320"/>
+      <c r="D320" t="n">
+        <v>0</v>
+      </c>
+      <c r="E320" t="n">
+        <v>0</v>
+      </c>
       <c r="F320" t="n">
         <v>7.62</v>
       </c>
@@ -20003,8 +20179,12 @@
       <c r="C322" t="n">
         <v>0.044</v>
       </c>
-      <c r="D322"/>
-      <c r="E322"/>
+      <c r="D322" t="n">
+        <v>0</v>
+      </c>
+      <c r="E322" t="n">
+        <v>0</v>
+      </c>
       <c r="F322" t="n">
         <v>12.08</v>
       </c>
@@ -20037,8 +20217,12 @@
       <c r="C323" t="n">
         <v>0.022</v>
       </c>
-      <c r="D323"/>
-      <c r="E323"/>
+      <c r="D323" t="n">
+        <v>0</v>
+      </c>
+      <c r="E323" t="n">
+        <v>0</v>
+      </c>
       <c r="F323" t="n">
         <v>6.71</v>
       </c>
@@ -20261,8 +20445,12 @@
       <c r="C329" t="n">
         <v>0.037</v>
       </c>
-      <c r="D329"/>
-      <c r="E329"/>
+      <c r="D329" t="n">
+        <v>0</v>
+      </c>
+      <c r="E329" t="n">
+        <v>0</v>
+      </c>
       <c r="F329" t="n">
         <v>8.06</v>
       </c>
@@ -21117,8 +21305,12 @@
       <c r="C352" t="n">
         <v>0.027</v>
       </c>
-      <c r="D352"/>
-      <c r="E352"/>
+      <c r="D352" t="n">
+        <v>0</v>
+      </c>
+      <c r="E352" t="n">
+        <v>0</v>
+      </c>
       <c r="F352" t="n">
         <v>6.64</v>
       </c>
@@ -21797,8 +21989,12 @@
       <c r="C370" t="n">
         <v>0.056</v>
       </c>
-      <c r="D370"/>
-      <c r="E370"/>
+      <c r="D370" t="n">
+        <v>0</v>
+      </c>
+      <c r="E370" t="n">
+        <v>0</v>
+      </c>
       <c r="F370" t="n">
         <v>9.33</v>
       </c>
@@ -23755,8 +23951,12 @@
       <c r="C422" t="n">
         <v>0.053</v>
       </c>
-      <c r="D422"/>
-      <c r="E422"/>
+      <c r="D422" t="n">
+        <v>0</v>
+      </c>
+      <c r="E422" t="n">
+        <v>0</v>
+      </c>
       <c r="F422" t="n">
         <v>7.44</v>
       </c>
@@ -23903,8 +24103,12 @@
       <c r="C426" t="n">
         <v>0.044</v>
       </c>
-      <c r="D426"/>
-      <c r="E426"/>
+      <c r="D426" t="n">
+        <v>0</v>
+      </c>
+      <c r="E426" t="n">
+        <v>0</v>
+      </c>
       <c r="F426" t="n">
         <v>7.84</v>
       </c>
@@ -23937,8 +24141,12 @@
       <c r="C427" t="n">
         <v>0.013</v>
       </c>
-      <c r="D427"/>
-      <c r="E427"/>
+      <c r="D427" t="n">
+        <v>0</v>
+      </c>
+      <c r="E427" t="n">
+        <v>0</v>
+      </c>
       <c r="F427" t="n">
         <v>8.21</v>
       </c>
@@ -24313,8 +24521,12 @@
       <c r="C437" t="n">
         <v>0.079</v>
       </c>
-      <c r="D437"/>
-      <c r="E437"/>
+      <c r="D437" t="n">
+        <v>0</v>
+      </c>
+      <c r="E437" t="n">
+        <v>0</v>
+      </c>
       <c r="F437" t="n">
         <v>7.51</v>
       </c>
@@ -24423,8 +24635,12 @@
       <c r="C440" t="n">
         <v>0.005</v>
       </c>
-      <c r="D440"/>
-      <c r="E440"/>
+      <c r="D440" t="n">
+        <v>0</v>
+      </c>
+      <c r="E440" t="n">
+        <v>0</v>
+      </c>
       <c r="F440" t="n">
         <v>7.9</v>
       </c>
@@ -25065,8 +25281,12 @@
       <c r="C457" t="n">
         <v>0.051</v>
       </c>
-      <c r="D457"/>
-      <c r="E457"/>
+      <c r="D457" t="n">
+        <v>0</v>
+      </c>
+      <c r="E457" t="n">
+        <v>0</v>
+      </c>
       <c r="F457" t="n">
         <v>6.76</v>
       </c>
@@ -26007,8 +26227,12 @@
       <c r="C483" t="n">
         <v>0.093</v>
       </c>
-      <c r="D483"/>
-      <c r="E483"/>
+      <c r="D483" t="n">
+        <v>0</v>
+      </c>
+      <c r="E483" t="n">
+        <v>0</v>
+      </c>
       <c r="F483" t="n">
         <v>8.45</v>
       </c>
@@ -26041,8 +26265,12 @@
       <c r="C484" t="n">
         <v>0.043</v>
       </c>
-      <c r="D484"/>
-      <c r="E484"/>
+      <c r="D484" t="n">
+        <v>0</v>
+      </c>
+      <c r="E484" t="n">
+        <v>0</v>
+      </c>
       <c r="F484" t="n">
         <v>6.61</v>
       </c>
@@ -26341,8 +26569,12 @@
       <c r="C492" t="n">
         <v>0.071</v>
       </c>
-      <c r="D492"/>
-      <c r="E492"/>
+      <c r="D492" t="n">
+        <v>0</v>
+      </c>
+      <c r="E492" t="n">
+        <v>0</v>
+      </c>
       <c r="F492" t="n">
         <v>9.59</v>
       </c>
@@ -26375,8 +26607,12 @@
       <c r="C493" t="n">
         <v>0.046</v>
       </c>
-      <c r="D493"/>
-      <c r="E493"/>
+      <c r="D493" t="n">
+        <v>0</v>
+      </c>
+      <c r="E493" t="n">
+        <v>0</v>
+      </c>
       <c r="F493" t="n">
         <v>8.11</v>
       </c>
@@ -26409,8 +26645,12 @@
       <c r="C494" t="n">
         <v>0.058</v>
       </c>
-      <c r="D494"/>
-      <c r="E494"/>
+      <c r="D494" t="n">
+        <v>0</v>
+      </c>
+      <c r="E494" t="n">
+        <v>0</v>
+      </c>
       <c r="F494" t="n">
         <v>7.44</v>
       </c>
@@ -26557,8 +26797,12 @@
       <c r="C498" t="n">
         <v>0.067</v>
       </c>
-      <c r="D498"/>
-      <c r="E498"/>
+      <c r="D498" t="n">
+        <v>0</v>
+      </c>
+      <c r="E498" t="n">
+        <v>0</v>
+      </c>
       <c r="F498" t="n">
         <v>6.38</v>
       </c>
@@ -26995,8 +27239,12 @@
       <c r="C510" t="n">
         <v>0.099</v>
       </c>
-      <c r="D510"/>
-      <c r="E510"/>
+      <c r="D510" t="n">
+        <v>0</v>
+      </c>
+      <c r="E510" t="n">
+        <v>0</v>
+      </c>
       <c r="F510" t="n">
         <v>8.97</v>
       </c>
@@ -27029,8 +27277,12 @@
       <c r="C511" t="n">
         <v>0.054</v>
       </c>
-      <c r="D511"/>
-      <c r="E511"/>
+      <c r="D511" t="n">
+        <v>0</v>
+      </c>
+      <c r="E511" t="n">
+        <v>0</v>
+      </c>
       <c r="F511" t="n">
         <v>7.33</v>
       </c>
@@ -27063,8 +27315,12 @@
       <c r="C512" t="n">
         <v>0.027</v>
       </c>
-      <c r="D512"/>
-      <c r="E512"/>
+      <c r="D512" t="n">
+        <v>0</v>
+      </c>
+      <c r="E512" t="n">
+        <v>0</v>
+      </c>
       <c r="F512" t="n">
         <v>7.54</v>
       </c>
@@ -27725,8 +27981,12 @@
       <c r="C531" t="n">
         <v>0.093</v>
       </c>
-      <c r="D531"/>
-      <c r="E531"/>
+      <c r="D531" t="n">
+        <v>0</v>
+      </c>
+      <c r="E531" t="n">
+        <v>0</v>
+      </c>
       <c r="F531" t="n">
         <v>8.01</v>
       </c>
@@ -27797,8 +28057,12 @@
       <c r="C533" t="n">
         <v>0.072</v>
       </c>
-      <c r="D533"/>
-      <c r="E533"/>
+      <c r="D533" t="n">
+        <v>0</v>
+      </c>
+      <c r="E533" t="n">
+        <v>0</v>
+      </c>
       <c r="F533" t="n">
         <v>5.92</v>
       </c>
@@ -27869,8 +28133,12 @@
       <c r="C535" t="n">
         <v>0.032</v>
       </c>
-      <c r="D535"/>
-      <c r="E535"/>
+      <c r="D535" t="n">
+        <v>0</v>
+      </c>
+      <c r="E535" t="n">
+        <v>0</v>
+      </c>
       <c r="F535" t="n">
         <v>6.47</v>
       </c>
@@ -27903,8 +28171,12 @@
       <c r="C536" t="n">
         <v>0.055</v>
       </c>
-      <c r="D536"/>
-      <c r="E536"/>
+      <c r="D536" t="n">
+        <v>0</v>
+      </c>
+      <c r="E536" t="n">
+        <v>0</v>
+      </c>
       <c r="F536" t="n">
         <v>9.21</v>
       </c>
@@ -28241,8 +28513,12 @@
       <c r="C545" t="n">
         <v>0.083</v>
       </c>
-      <c r="D545"/>
-      <c r="E545"/>
+      <c r="D545" t="n">
+        <v>0</v>
+      </c>
+      <c r="E545" t="n">
+        <v>0</v>
+      </c>
       <c r="F545" t="n">
         <v>11.64</v>
       </c>
@@ -28389,8 +28665,12 @@
       <c r="C549" t="n">
         <v>0.034</v>
       </c>
-      <c r="D549"/>
-      <c r="E549"/>
+      <c r="D549" t="n">
+        <v>0</v>
+      </c>
+      <c r="E549" t="n">
+        <v>0</v>
+      </c>
       <c r="F549" t="n">
         <v>8.43</v>
       </c>
@@ -28993,8 +29273,12 @@
       <c r="C565" t="n">
         <v>0.031</v>
       </c>
-      <c r="D565"/>
-      <c r="E565"/>
+      <c r="D565" t="n">
+        <v>0</v>
+      </c>
+      <c r="E565" t="n">
+        <v>0</v>
+      </c>
       <c r="F565" t="n">
         <v>7.09</v>
       </c>
@@ -29407,8 +29691,12 @@
       <c r="C576" t="n">
         <v>0.018</v>
       </c>
-      <c r="D576"/>
-      <c r="E576"/>
+      <c r="D576" t="n">
+        <v>0</v>
+      </c>
+      <c r="E576" t="n">
+        <v>0</v>
+      </c>
       <c r="F576" t="n">
         <v>11.48</v>
       </c>
@@ -29441,8 +29729,12 @@
       <c r="C577" t="n">
         <v>0.056</v>
       </c>
-      <c r="D577"/>
-      <c r="E577"/>
+      <c r="D577" t="n">
+        <v>0</v>
+      </c>
+      <c r="E577" t="n">
+        <v>0</v>
+      </c>
       <c r="F577" t="n">
         <v>6.47</v>
       </c>
@@ -29551,8 +29843,12 @@
       <c r="C580" t="n">
         <v>0.044</v>
       </c>
-      <c r="D580"/>
-      <c r="E580"/>
+      <c r="D580" t="n">
+        <v>0</v>
+      </c>
+      <c r="E580" t="n">
+        <v>0</v>
+      </c>
       <c r="F580" t="n">
         <v>7.42</v>
       </c>
@@ -29585,8 +29881,12 @@
       <c r="C581" t="n">
         <v>0.025</v>
       </c>
-      <c r="D581"/>
-      <c r="E581"/>
+      <c r="D581" t="n">
+        <v>0</v>
+      </c>
+      <c r="E581" t="n">
+        <v>0</v>
+      </c>
       <c r="F581" t="n">
         <v>6.94</v>
       </c>
@@ -30061,8 +30361,12 @@
       <c r="C594" t="n">
         <v>0.092</v>
       </c>
-      <c r="D594"/>
-      <c r="E594"/>
+      <c r="D594" t="n">
+        <v>0</v>
+      </c>
+      <c r="E594" t="n">
+        <v>0</v>
+      </c>
       <c r="F594" t="n">
         <v>7.1</v>
       </c>
@@ -30171,8 +30475,12 @@
       <c r="C597" t="n">
         <v>0.136</v>
       </c>
-      <c r="D597"/>
-      <c r="E597"/>
+      <c r="D597" t="n">
+        <v>0</v>
+      </c>
+      <c r="E597" t="n">
+        <v>0</v>
+      </c>
       <c r="F597" t="n">
         <v>7.47</v>
       </c>
@@ -30205,8 +30513,12 @@
       <c r="C598" t="n">
         <v>0.044</v>
       </c>
-      <c r="D598"/>
-      <c r="E598"/>
+      <c r="D598" t="n">
+        <v>0</v>
+      </c>
+      <c r="E598" t="n">
+        <v>0</v>
+      </c>
       <c r="F598" t="n">
         <v>7.49</v>
       </c>
@@ -30239,8 +30551,12 @@
       <c r="C599" t="n">
         <v>0.08</v>
       </c>
-      <c r="D599"/>
-      <c r="E599"/>
+      <c r="D599" t="n">
+        <v>0</v>
+      </c>
+      <c r="E599" t="n">
+        <v>0</v>
+      </c>
       <c r="F599" t="n">
         <v>2.81</v>
       </c>
@@ -30311,8 +30627,12 @@
       <c r="C601" t="n">
         <v>0.073</v>
       </c>
-      <c r="D601"/>
-      <c r="E601"/>
+      <c r="D601" t="n">
+        <v>0</v>
+      </c>
+      <c r="E601" t="n">
+        <v>0</v>
+      </c>
       <c r="F601" t="n">
         <v>4.23</v>
       </c>
@@ -30383,8 +30703,12 @@
       <c r="C603" t="n">
         <v>0.06</v>
       </c>
-      <c r="D603"/>
-      <c r="E603"/>
+      <c r="D603" t="n">
+        <v>0</v>
+      </c>
+      <c r="E603" t="n">
+        <v>0</v>
+      </c>
       <c r="F603" t="n">
         <v>4.47</v>
       </c>
@@ -30897,8 +31221,12 @@
       <c r="C617" t="n">
         <v>0.075</v>
       </c>
-      <c r="D617"/>
-      <c r="E617"/>
+      <c r="D617" t="n">
+        <v>0</v>
+      </c>
+      <c r="E617" t="n">
+        <v>0</v>
+      </c>
       <c r="F617" t="n">
         <v>17.35</v>
       </c>
@@ -31007,8 +31335,12 @@
       <c r="C620" t="n">
         <v>0.109</v>
       </c>
-      <c r="D620"/>
-      <c r="E620"/>
+      <c r="D620" t="n">
+        <v>0</v>
+      </c>
+      <c r="E620" t="n">
+        <v>0</v>
+      </c>
       <c r="F620" t="n">
         <v>7.07</v>
       </c>
@@ -31079,8 +31411,12 @@
       <c r="C622" t="n">
         <v>0.107</v>
       </c>
-      <c r="D622"/>
-      <c r="E622"/>
+      <c r="D622" t="n">
+        <v>0</v>
+      </c>
+      <c r="E622" t="n">
+        <v>0</v>
+      </c>
       <c r="F622" t="n">
         <v>7.12</v>
       </c>
@@ -31189,8 +31525,12 @@
       <c r="C625" t="n">
         <v>0.065</v>
       </c>
-      <c r="D625"/>
-      <c r="E625"/>
+      <c r="D625" t="n">
+        <v>0</v>
+      </c>
+      <c r="E625" t="n">
+        <v>0</v>
+      </c>
       <c r="F625" t="n">
         <v>8.27</v>
       </c>
@@ -31261,8 +31601,12 @@
       <c r="C627" t="n">
         <v>0.094</v>
       </c>
-      <c r="D627"/>
-      <c r="E627"/>
+      <c r="D627" t="n">
+        <v>0</v>
+      </c>
+      <c r="E627" t="n">
+        <v>0</v>
+      </c>
       <c r="F627" t="n">
         <v>9.58</v>
       </c>
@@ -31675,8 +32019,12 @@
       <c r="C638" t="n">
         <v>0.063</v>
       </c>
-      <c r="D638"/>
-      <c r="E638"/>
+      <c r="D638" t="n">
+        <v>0</v>
+      </c>
+      <c r="E638" t="n">
+        <v>0</v>
+      </c>
       <c r="F638" t="n">
         <v>2.59</v>
       </c>
@@ -31785,8 +32133,12 @@
       <c r="C641" t="n">
         <v>0.128</v>
       </c>
-      <c r="D641"/>
-      <c r="E641"/>
+      <c r="D641" t="n">
+        <v>0</v>
+      </c>
+      <c r="E641" t="n">
+        <v>0</v>
+      </c>
       <c r="F641" t="n">
         <v>7.15</v>
       </c>
@@ -32313,8 +32665,12 @@
       <c r="C655" t="n">
         <v>0.063</v>
       </c>
-      <c r="D655"/>
-      <c r="E655"/>
+      <c r="D655" t="n">
+        <v>0</v>
+      </c>
+      <c r="E655" t="n">
+        <v>0</v>
+      </c>
       <c r="F655" t="n">
         <v>6.46</v>
       </c>
@@ -32347,8 +32703,12 @@
       <c r="C656" t="n">
         <v>0.072</v>
       </c>
-      <c r="D656"/>
-      <c r="E656"/>
+      <c r="D656" t="n">
+        <v>0</v>
+      </c>
+      <c r="E656" t="n">
+        <v>0</v>
+      </c>
       <c r="F656" t="n">
         <v>6.08</v>
       </c>
@@ -32419,8 +32779,12 @@
       <c r="C658" t="n">
         <v>0.047</v>
       </c>
-      <c r="D658"/>
-      <c r="E658"/>
+      <c r="D658" t="n">
+        <v>0</v>
+      </c>
+      <c r="E658" t="n">
+        <v>0</v>
+      </c>
       <c r="F658" t="n">
         <v>7.82</v>
       </c>
@@ -32643,8 +33007,12 @@
       <c r="C664" t="n">
         <v>0.066</v>
       </c>
-      <c r="D664"/>
-      <c r="E664"/>
+      <c r="D664" t="n">
+        <v>0</v>
+      </c>
+      <c r="E664" t="n">
+        <v>0</v>
+      </c>
       <c r="F664" t="n">
         <v>19.44</v>
       </c>
@@ -32753,8 +33121,12 @@
       <c r="C667" t="n">
         <v>0.06</v>
       </c>
-      <c r="D667"/>
-      <c r="E667"/>
+      <c r="D667" t="n">
+        <v>0</v>
+      </c>
+      <c r="E667" t="n">
+        <v>0</v>
+      </c>
       <c r="F667" t="n">
         <v>7.47</v>
       </c>
@@ -32787,8 +33159,12 @@
       <c r="C668" t="n">
         <v>0.07</v>
       </c>
-      <c r="D668"/>
-      <c r="E668"/>
+      <c r="D668" t="n">
+        <v>0</v>
+      </c>
+      <c r="E668" t="n">
+        <v>0</v>
+      </c>
       <c r="F668" t="n">
         <v>6.71</v>
       </c>
@@ -33315,8 +33691,12 @@
       <c r="C682" t="n">
         <v>0.062</v>
       </c>
-      <c r="D682"/>
-      <c r="E682"/>
+      <c r="D682" t="n">
+        <v>0</v>
+      </c>
+      <c r="E682" t="n">
+        <v>0</v>
+      </c>
       <c r="F682" t="n">
         <v>6.09</v>
       </c>
@@ -33729,8 +34109,12 @@
       <c r="C693" t="n">
         <v>0.017</v>
       </c>
-      <c r="D693"/>
-      <c r="E693"/>
+      <c r="D693" t="n">
+        <v>0</v>
+      </c>
+      <c r="E693" t="n">
+        <v>0</v>
+      </c>
       <c r="F693"/>
       <c r="G693"/>
       <c r="H693"/>
@@ -33939,8 +34323,12 @@
       <c r="C699" t="n">
         <v>0.007</v>
       </c>
-      <c r="D699"/>
-      <c r="E699"/>
+      <c r="D699" t="n">
+        <v>0</v>
+      </c>
+      <c r="E699" t="n">
+        <v>0</v>
+      </c>
       <c r="F699"/>
       <c r="G699"/>
       <c r="H699"/>
@@ -33994,7 +34382,9 @@
       <c r="B701" t="n">
         <v>94.374</v>
       </c>
-      <c r="C701"/>
+      <c r="C701" t="n">
+        <v>0</v>
+      </c>
       <c r="D701" t="n">
         <v>52.5</v>
       </c>
@@ -34551,8 +34941,12 @@
       <c r="C716" t="n">
         <v>0</v>
       </c>
-      <c r="D716"/>
-      <c r="E716"/>
+      <c r="D716" t="n">
+        <v>0</v>
+      </c>
+      <c r="E716" t="n">
+        <v>0</v>
+      </c>
       <c r="F716" t="n">
         <v>8.75</v>
       </c>
@@ -34965,8 +35359,12 @@
       <c r="C727" t="n">
         <v>0.012</v>
       </c>
-      <c r="D727"/>
-      <c r="E727"/>
+      <c r="D727" t="n">
+        <v>0</v>
+      </c>
+      <c r="E727" t="n">
+        <v>0</v>
+      </c>
       <c r="F727" t="n">
         <v>9.31</v>
       </c>
@@ -37151,8 +37549,12 @@
       <c r="C785" t="n">
         <v>0.002</v>
       </c>
-      <c r="D785"/>
-      <c r="E785"/>
+      <c r="D785" t="n">
+        <v>0</v>
+      </c>
+      <c r="E785" t="n">
+        <v>0</v>
+      </c>
       <c r="F785" t="n">
         <v>8.13</v>
       </c>
@@ -37182,7 +37584,9 @@
       <c r="B786" t="n">
         <v>92.166</v>
       </c>
-      <c r="C786"/>
+      <c r="C786" t="n">
+        <v>0</v>
+      </c>
       <c r="D786" t="n">
         <v>149.4</v>
       </c>
@@ -37297,8 +37701,12 @@
       <c r="C789" t="n">
         <v>0.004</v>
       </c>
-      <c r="D789"/>
-      <c r="E789"/>
+      <c r="D789" t="n">
+        <v>0</v>
+      </c>
+      <c r="E789" t="n">
+        <v>0</v>
+      </c>
       <c r="F789" t="n">
         <v>8.62</v>
       </c>
@@ -37711,8 +38119,12 @@
       <c r="C800" t="n">
         <v>0.072</v>
       </c>
-      <c r="D800"/>
-      <c r="E800"/>
+      <c r="D800" t="n">
+        <v>0</v>
+      </c>
+      <c r="E800" t="n">
+        <v>0</v>
+      </c>
       <c r="F800" t="n">
         <v>8.08</v>
       </c>
@@ -37821,8 +38233,12 @@
       <c r="C803" t="n">
         <v>0.013</v>
       </c>
-      <c r="D803"/>
-      <c r="E803"/>
+      <c r="D803" t="n">
+        <v>0</v>
+      </c>
+      <c r="E803" t="n">
+        <v>0</v>
+      </c>
       <c r="F803" t="n">
         <v>8.52</v>
       </c>
@@ -38235,8 +38651,12 @@
       <c r="C814" t="n">
         <v>0.006</v>
       </c>
-      <c r="D814"/>
-      <c r="E814"/>
+      <c r="D814" t="n">
+        <v>0</v>
+      </c>
+      <c r="E814" t="n">
+        <v>0</v>
+      </c>
       <c r="F814" t="n">
         <v>7.88</v>
       </c>
@@ -39115,8 +39535,12 @@
       <c r="C838" t="n">
         <v>0.096</v>
       </c>
-      <c r="D838"/>
-      <c r="E838"/>
+      <c r="D838" t="n">
+        <v>0</v>
+      </c>
+      <c r="E838" t="n">
+        <v>0</v>
+      </c>
       <c r="F838"/>
       <c r="G838"/>
       <c r="H838"/>
@@ -39539,8 +39963,12 @@
       <c r="C850" t="n">
         <v>0.031</v>
       </c>
-      <c r="D850"/>
-      <c r="E850"/>
+      <c r="D850" t="n">
+        <v>0</v>
+      </c>
+      <c r="E850" t="n">
+        <v>0</v>
+      </c>
       <c r="F850" t="n">
         <v>8.38</v>
       </c>
@@ -40257,8 +40685,12 @@
       <c r="C869" t="n">
         <v>0.019</v>
       </c>
-      <c r="D869"/>
-      <c r="E869"/>
+      <c r="D869" t="n">
+        <v>0</v>
+      </c>
+      <c r="E869" t="n">
+        <v>0</v>
+      </c>
       <c r="F869" t="n">
         <v>8.8</v>
       </c>
@@ -40291,8 +40723,12 @@
       <c r="C870" t="n">
         <v>0.013</v>
       </c>
-      <c r="D870"/>
-      <c r="E870"/>
+      <c r="D870" t="n">
+        <v>0</v>
+      </c>
+      <c r="E870" t="n">
+        <v>0</v>
+      </c>
       <c r="F870" t="n">
         <v>6.95</v>
       </c>
@@ -40463,8 +40899,12 @@
       <c r="C875" t="n">
         <v>0.01</v>
       </c>
-      <c r="D875"/>
-      <c r="E875"/>
+      <c r="D875" t="n">
+        <v>0</v>
+      </c>
+      <c r="E875" t="n">
+        <v>0</v>
+      </c>
       <c r="F875" t="n">
         <v>8.79</v>
       </c>
@@ -40535,8 +40975,12 @@
       <c r="C877" t="n">
         <v>0.019</v>
       </c>
-      <c r="D877"/>
-      <c r="E877"/>
+      <c r="D877" t="n">
+        <v>0</v>
+      </c>
+      <c r="E877" t="n">
+        <v>0</v>
+      </c>
       <c r="F877" t="n">
         <v>9</v>
       </c>
@@ -40835,8 +41279,12 @@
       <c r="C885" t="n">
         <v>0.002</v>
       </c>
-      <c r="D885"/>
-      <c r="E885"/>
+      <c r="D885" t="n">
+        <v>0</v>
+      </c>
+      <c r="E885" t="n">
+        <v>0</v>
+      </c>
       <c r="F885" t="n">
         <v>9.58</v>
       </c>
@@ -40869,8 +41317,12 @@
       <c r="C886" t="n">
         <v>0.043</v>
       </c>
-      <c r="D886"/>
-      <c r="E886"/>
+      <c r="D886" t="n">
+        <v>0</v>
+      </c>
+      <c r="E886" t="n">
+        <v>0</v>
+      </c>
       <c r="F886" t="n">
         <v>6.59</v>
       </c>
@@ -41380,7 +41832,9 @@
       <c r="B900" t="n">
         <v>92.043</v>
       </c>
-      <c r="C900"/>
+      <c r="C900" t="n">
+        <v>0</v>
+      </c>
       <c r="D900" t="n">
         <v>468.5</v>
       </c>
@@ -41609,8 +42063,12 @@
       <c r="C906" t="n">
         <v>0.038</v>
       </c>
-      <c r="D906"/>
-      <c r="E906"/>
+      <c r="D906" t="n">
+        <v>0</v>
+      </c>
+      <c r="E906" t="n">
+        <v>0</v>
+      </c>
       <c r="F906" t="n">
         <v>8.1</v>
       </c>
@@ -41833,8 +42291,12 @@
       <c r="C912" t="n">
         <v>0.042</v>
       </c>
-      <c r="D912"/>
-      <c r="E912"/>
+      <c r="D912" t="n">
+        <v>0</v>
+      </c>
+      <c r="E912" t="n">
+        <v>0</v>
+      </c>
       <c r="F912" t="n">
         <v>7.79</v>
       </c>
@@ -41981,8 +42443,12 @@
       <c r="C916" t="n">
         <v>0.012</v>
       </c>
-      <c r="D916"/>
-      <c r="E916"/>
+      <c r="D916" t="n">
+        <v>0</v>
+      </c>
+      <c r="E916" t="n">
+        <v>0</v>
+      </c>
       <c r="F916" t="n">
         <v>8.68</v>
       </c>
@@ -42623,8 +43089,12 @@
       <c r="C933" t="n">
         <v>0.058</v>
       </c>
-      <c r="D933"/>
-      <c r="E933"/>
+      <c r="D933" t="n">
+        <v>0</v>
+      </c>
+      <c r="E933" t="n">
+        <v>0</v>
+      </c>
       <c r="F933" t="n">
         <v>7.66</v>
       </c>
@@ -42695,8 +43165,12 @@
       <c r="C935" t="n">
         <v>0.01</v>
       </c>
-      <c r="D935"/>
-      <c r="E935"/>
+      <c r="D935" t="n">
+        <v>0</v>
+      </c>
+      <c r="E935" t="n">
+        <v>0</v>
+      </c>
       <c r="F935" t="n">
         <v>4.59</v>
       </c>
@@ -43033,8 +43507,12 @@
       <c r="C944" t="n">
         <v>0.043</v>
       </c>
-      <c r="D944"/>
-      <c r="E944"/>
+      <c r="D944" t="n">
+        <v>0</v>
+      </c>
+      <c r="E944" t="n">
+        <v>0</v>
+      </c>
       <c r="F944" t="n">
         <v>9.74</v>
       </c>
@@ -43219,8 +43697,12 @@
       <c r="C949" t="n">
         <v>0.083</v>
       </c>
-      <c r="D949"/>
-      <c r="E949"/>
+      <c r="D949" t="n">
+        <v>0</v>
+      </c>
+      <c r="E949" t="n">
+        <v>0</v>
+      </c>
       <c r="F949" t="n">
         <v>14.04</v>
       </c>
@@ -43253,8 +43735,12 @@
       <c r="C950" t="n">
         <v>0.022</v>
       </c>
-      <c r="D950"/>
-      <c r="E950"/>
+      <c r="D950" t="n">
+        <v>0</v>
+      </c>
+      <c r="E950" t="n">
+        <v>0</v>
+      </c>
       <c r="F950" t="n">
         <v>8.22</v>
       </c>
@@ -44503,8 +44989,12 @@
       <c r="C983" t="n">
         <v>0.036</v>
       </c>
-      <c r="D983"/>
-      <c r="E983"/>
+      <c r="D983" t="n">
+        <v>0</v>
+      </c>
+      <c r="E983" t="n">
+        <v>0</v>
+      </c>
       <c r="F983" t="n">
         <v>7.95</v>
       </c>
@@ -44537,8 +45027,12 @@
       <c r="C984" t="n">
         <v>0.084</v>
       </c>
-      <c r="D984"/>
-      <c r="E984"/>
+      <c r="D984" t="n">
+        <v>0</v>
+      </c>
+      <c r="E984" t="n">
+        <v>0</v>
+      </c>
       <c r="F984" t="n">
         <v>15.32</v>
       </c>
@@ -44951,8 +45445,12 @@
       <c r="C995" t="n">
         <v>0.028</v>
       </c>
-      <c r="D995"/>
-      <c r="E995"/>
+      <c r="D995" t="n">
+        <v>0</v>
+      </c>
+      <c r="E995" t="n">
+        <v>0</v>
+      </c>
       <c r="F995" t="n">
         <v>7.09</v>
       </c>
@@ -45213,8 +45711,12 @@
       <c r="C1002" t="n">
         <v>0.065</v>
       </c>
-      <c r="D1002"/>
-      <c r="E1002"/>
+      <c r="D1002" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1002" t="n">
+        <v>0</v>
+      </c>
       <c r="F1002" t="n">
         <v>6.37</v>
       </c>
@@ -45247,8 +45749,12 @@
       <c r="C1003" t="n">
         <v>0.018</v>
       </c>
-      <c r="D1003"/>
-      <c r="E1003"/>
+      <c r="D1003" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1003" t="n">
+        <v>0</v>
+      </c>
       <c r="F1003" t="n">
         <v>8.05</v>
       </c>
@@ -45281,8 +45787,12 @@
       <c r="C1004" t="n">
         <v>0.053</v>
       </c>
-      <c r="D1004"/>
-      <c r="E1004"/>
+      <c r="D1004" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1004" t="n">
+        <v>0</v>
+      </c>
       <c r="F1004" t="n">
         <v>6.81</v>
       </c>
@@ -45429,8 +45939,12 @@
       <c r="C1008" t="n">
         <v>0.092</v>
       </c>
-      <c r="D1008"/>
-      <c r="E1008"/>
+      <c r="D1008" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1008" t="n">
+        <v>0</v>
+      </c>
       <c r="F1008" t="n">
         <v>7.75</v>
       </c>
@@ -45463,8 +45977,12 @@
       <c r="C1009" t="n">
         <v>0.051</v>
       </c>
-      <c r="D1009"/>
-      <c r="E1009"/>
+      <c r="D1009" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1009" t="n">
+        <v>0</v>
+      </c>
       <c r="F1009" t="n">
         <v>7.03</v>
       </c>
@@ -45573,8 +46091,12 @@
       <c r="C1012" t="n">
         <v>0.017</v>
       </c>
-      <c r="D1012"/>
-      <c r="E1012"/>
+      <c r="D1012" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1012" t="n">
+        <v>0</v>
+      </c>
       <c r="F1012" t="n">
         <v>6.52</v>
       </c>
@@ -45987,8 +46509,12 @@
       <c r="C1023" t="n">
         <v>0.052</v>
       </c>
-      <c r="D1023"/>
-      <c r="E1023"/>
+      <c r="D1023" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1023" t="n">
+        <v>0</v>
+      </c>
       <c r="F1023" t="n">
         <v>6.69</v>
       </c>
@@ -46995,8 +47521,12 @@
       <c r="C1050" t="n">
         <v>0.011</v>
       </c>
-      <c r="D1050"/>
-      <c r="E1050"/>
+      <c r="D1050" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1050" t="n">
+        <v>0</v>
+      </c>
       <c r="F1050" t="n">
         <v>8.47</v>
       </c>
@@ -47067,8 +47597,12 @@
       <c r="C1052" t="n">
         <v>0.126</v>
       </c>
-      <c r="D1052"/>
-      <c r="E1052"/>
+      <c r="D1052" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1052" t="n">
+        <v>0</v>
+      </c>
       <c r="F1052" t="n">
         <v>8.3</v>
       </c>
@@ -47515,8 +48049,12 @@
       <c r="C1065" t="n">
         <v>0.269</v>
       </c>
-      <c r="D1065"/>
-      <c r="E1065"/>
+      <c r="D1065" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1065" t="n">
+        <v>0</v>
+      </c>
       <c r="F1065" t="n">
         <v>4.43</v>
       </c>
@@ -47663,8 +48201,12 @@
       <c r="C1069" t="n">
         <v>0.154</v>
       </c>
-      <c r="D1069"/>
-      <c r="E1069"/>
+      <c r="D1069" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1069" t="n">
+        <v>0</v>
+      </c>
       <c r="F1069" t="n">
         <v>9</v>
       </c>
@@ -47797,8 +48339,12 @@
       <c r="C1073" t="n">
         <v>0.044</v>
       </c>
-      <c r="D1073"/>
-      <c r="E1073"/>
+      <c r="D1073" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1073" t="n">
+        <v>0</v>
+      </c>
       <c r="F1073" t="n">
         <v>8.21</v>
       </c>
@@ -48487,8 +49033,12 @@
       <c r="C1092" t="n">
         <v>0.008</v>
       </c>
-      <c r="D1092"/>
-      <c r="E1092"/>
+      <c r="D1092" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1092" t="n">
+        <v>0</v>
+      </c>
       <c r="F1092" t="n">
         <v>8.17</v>
       </c>
@@ -48711,8 +49261,12 @@
       <c r="C1098" t="n">
         <v>0.07</v>
       </c>
-      <c r="D1098"/>
-      <c r="E1098"/>
+      <c r="D1098" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1098" t="n">
+        <v>0</v>
+      </c>
       <c r="F1098" t="n">
         <v>9.57</v>
       </c>
@@ -49201,8 +49755,12 @@
       <c r="C1111" t="n">
         <v>0.023</v>
       </c>
-      <c r="D1111"/>
-      <c r="E1111"/>
+      <c r="D1111" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1111" t="n">
+        <v>0</v>
+      </c>
       <c r="F1111" t="n">
         <v>8.14</v>
       </c>
@@ -49501,8 +50059,12 @@
       <c r="C1119" t="n">
         <v>0.025</v>
       </c>
-      <c r="D1119"/>
-      <c r="E1119"/>
+      <c r="D1119" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1119" t="n">
+        <v>0</v>
+      </c>
       <c r="F1119" t="n">
         <v>9.03</v>
       </c>
@@ -49763,8 +50325,12 @@
       <c r="C1126" t="n">
         <v>0.04</v>
       </c>
-      <c r="D1126"/>
-      <c r="E1126"/>
+      <c r="D1126" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1126" t="n">
+        <v>0</v>
+      </c>
       <c r="F1126" t="n">
         <v>10.26</v>
       </c>
@@ -50277,8 +50843,12 @@
       <c r="C1140" t="n">
         <v>0.026</v>
       </c>
-      <c r="D1140"/>
-      <c r="E1140"/>
+      <c r="D1140" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1140" t="n">
+        <v>0</v>
+      </c>
       <c r="F1140" t="n">
         <v>20.5</v>
       </c>
@@ -50387,8 +50957,12 @@
       <c r="C1143" t="n">
         <v>0.033</v>
       </c>
-      <c r="D1143"/>
-      <c r="E1143"/>
+      <c r="D1143" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1143" t="n">
+        <v>0</v>
+      </c>
       <c r="F1143" t="n">
         <v>9.91</v>
       </c>
@@ -50749,8 +51323,12 @@
       <c r="C1153" t="n">
         <v>0.025</v>
       </c>
-      <c r="D1153"/>
-      <c r="E1153"/>
+      <c r="D1153" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1153" t="n">
+        <v>0</v>
+      </c>
       <c r="F1153" t="n">
         <v>15.53</v>
       </c>
@@ -50821,8 +51399,12 @@
       <c r="C1155" t="n">
         <v>0.01</v>
       </c>
-      <c r="D1155"/>
-      <c r="E1155"/>
+      <c r="D1155" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1155" t="n">
+        <v>0</v>
+      </c>
       <c r="F1155" t="n">
         <v>18.21</v>
       </c>
@@ -50855,8 +51437,12 @@
       <c r="C1156" t="n">
         <v>0.037</v>
       </c>
-      <c r="D1156"/>
-      <c r="E1156"/>
+      <c r="D1156" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1156" t="n">
+        <v>0</v>
+      </c>
       <c r="F1156" t="n">
         <v>10.95</v>
       </c>
@@ -50889,8 +51475,12 @@
       <c r="C1157" t="n">
         <v>0.027</v>
       </c>
-      <c r="D1157"/>
-      <c r="E1157"/>
+      <c r="D1157" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1157" t="n">
+        <v>0</v>
+      </c>
       <c r="F1157" t="n">
         <v>10.86</v>
       </c>
@@ -51113,8 +51703,12 @@
       <c r="C1163" t="n">
         <v>0.06</v>
       </c>
-      <c r="D1163"/>
-      <c r="E1163"/>
+      <c r="D1163" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1163" t="n">
+        <v>0</v>
+      </c>
       <c r="F1163" t="n">
         <v>6.38</v>
       </c>
@@ -51551,8 +52145,12 @@
       <c r="C1175" t="n">
         <v>0.044</v>
       </c>
-      <c r="D1175"/>
-      <c r="E1175"/>
+      <c r="D1175" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1175" t="n">
+        <v>0</v>
+      </c>
       <c r="F1175" t="n">
         <v>6.33</v>
       </c>
@@ -51889,8 +52487,12 @@
       <c r="C1184" t="n">
         <v>0.115</v>
       </c>
-      <c r="D1184"/>
-      <c r="E1184"/>
+      <c r="D1184" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1184" t="n">
+        <v>0</v>
+      </c>
       <c r="F1184" t="n">
         <v>7.18</v>
       </c>
@@ -51923,8 +52525,12 @@
       <c r="C1185" t="n">
         <v>0.049</v>
       </c>
-      <c r="D1185"/>
-      <c r="E1185"/>
+      <c r="D1185" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1185" t="n">
+        <v>0</v>
+      </c>
       <c r="F1185" t="n">
         <v>5.85</v>
       </c>
@@ -51957,8 +52563,12 @@
       <c r="C1186" t="n">
         <v>0.045</v>
       </c>
-      <c r="D1186"/>
-      <c r="E1186"/>
+      <c r="D1186" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1186" t="n">
+        <v>0</v>
+      </c>
       <c r="F1186" t="n">
         <v>6.4</v>
       </c>
@@ -51991,8 +52601,12 @@
       <c r="C1187" t="n">
         <v>0.049</v>
       </c>
-      <c r="D1187"/>
-      <c r="E1187"/>
+      <c r="D1187" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1187" t="n">
+        <v>0</v>
+      </c>
       <c r="F1187" t="n">
         <v>9.03</v>
       </c>
@@ -52671,8 +53285,12 @@
       <c r="C1205" t="n">
         <v>0.041</v>
       </c>
-      <c r="D1205"/>
-      <c r="E1205"/>
+      <c r="D1205" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1205" t="n">
+        <v>0</v>
+      </c>
       <c r="F1205" t="n">
         <v>17.24</v>
       </c>
@@ -52857,8 +53475,12 @@
       <c r="C1210" t="n">
         <v>0.032</v>
       </c>
-      <c r="D1210"/>
-      <c r="E1210"/>
+      <c r="D1210" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1210" t="n">
+        <v>0</v>
+      </c>
       <c r="F1210" t="n">
         <v>10.64</v>
       </c>
@@ -53575,8 +54197,12 @@
       <c r="C1229" t="n">
         <v>0.07</v>
       </c>
-      <c r="D1229"/>
-      <c r="E1229"/>
+      <c r="D1229" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1229" t="n">
+        <v>0</v>
+      </c>
       <c r="F1229" t="n">
         <v>8.44</v>
       </c>
@@ -54103,8 +54729,12 @@
       <c r="C1243" t="n">
         <v>0.034</v>
       </c>
-      <c r="D1243"/>
-      <c r="E1243"/>
+      <c r="D1243" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1243" t="n">
+        <v>0</v>
+      </c>
       <c r="F1243" t="n">
         <v>7.43</v>
       </c>
@@ -54213,8 +54843,12 @@
       <c r="C1246" t="n">
         <v>0.051</v>
       </c>
-      <c r="D1246"/>
-      <c r="E1246"/>
+      <c r="D1246" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1246" t="n">
+        <v>0</v>
+      </c>
       <c r="F1246" t="n">
         <v>7.56</v>
       </c>
@@ -54247,8 +54881,12 @@
       <c r="C1247" t="n">
         <v>0.032</v>
       </c>
-      <c r="D1247"/>
-      <c r="E1247"/>
+      <c r="D1247" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1247" t="n">
+        <v>0</v>
+      </c>
       <c r="F1247" t="n">
         <v>7.85</v>
       </c>
@@ -54975,8 +55613,12 @@
       <c r="C1267" t="n">
         <v>0.078</v>
       </c>
-      <c r="D1267"/>
-      <c r="E1267"/>
+      <c r="D1267" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1267" t="n">
+        <v>0</v>
+      </c>
       <c r="F1267" t="n">
         <v>7.69</v>
       </c>
@@ -55199,8 +55841,12 @@
       <c r="C1273" t="n">
         <v>0.083</v>
       </c>
-      <c r="D1273"/>
-      <c r="E1273"/>
+      <c r="D1273" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1273" t="n">
+        <v>0</v>
+      </c>
       <c r="F1273" t="n">
         <v>8.44</v>
       </c>
@@ -55385,8 +56031,12 @@
       <c r="C1278" t="n">
         <v>0.137</v>
       </c>
-      <c r="D1278"/>
-      <c r="E1278"/>
+      <c r="D1278" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1278" t="n">
+        <v>0</v>
+      </c>
       <c r="F1278" t="n">
         <v>12.46</v>
       </c>
@@ -55533,8 +56183,12 @@
       <c r="C1282" t="n">
         <v>0.038</v>
       </c>
-      <c r="D1282"/>
-      <c r="E1282"/>
+      <c r="D1282" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1282" t="n">
+        <v>0</v>
+      </c>
       <c r="F1282" t="n">
         <v>6.09</v>
       </c>
@@ -55567,8 +56221,12 @@
       <c r="C1283" t="n">
         <v>0.047</v>
       </c>
-      <c r="D1283"/>
-      <c r="E1283"/>
+      <c r="D1283" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1283" t="n">
+        <v>0</v>
+      </c>
       <c r="F1283" t="n">
         <v>7.02</v>
       </c>
@@ -56019,8 +56677,12 @@
       <c r="C1295" t="n">
         <v>0.033</v>
       </c>
-      <c r="D1295"/>
-      <c r="E1295"/>
+      <c r="D1295" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1295" t="n">
+        <v>0</v>
+      </c>
       <c r="F1295" t="n">
         <v>8.38</v>
       </c>
@@ -56053,8 +56715,12 @@
       <c r="C1296" t="n">
         <v>0.017</v>
       </c>
-      <c r="D1296"/>
-      <c r="E1296"/>
+      <c r="D1296" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1296" t="n">
+        <v>0</v>
+      </c>
       <c r="F1296" t="n">
         <v>8.68</v>
       </c>
@@ -56163,8 +56829,12 @@
       <c r="C1299" t="n">
         <v>0.031</v>
       </c>
-      <c r="D1299"/>
-      <c r="E1299"/>
+      <c r="D1299" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1299" t="n">
+        <v>0</v>
+      </c>
       <c r="F1299" t="n">
         <v>7.53</v>
       </c>
@@ -56387,8 +57057,12 @@
       <c r="C1305" t="n">
         <v>0.02</v>
       </c>
-      <c r="D1305"/>
-      <c r="E1305"/>
+      <c r="D1305" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1305" t="n">
+        <v>0</v>
+      </c>
       <c r="F1305" t="n">
         <v>11.56</v>
       </c>
@@ -56725,8 +57399,12 @@
       <c r="C1314" t="n">
         <v>0.059</v>
       </c>
-      <c r="D1314"/>
-      <c r="E1314"/>
+      <c r="D1314" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1314" t="n">
+        <v>0</v>
+      </c>
       <c r="F1314" t="n">
         <v>7.63</v>
       </c>
@@ -56873,8 +57551,12 @@
       <c r="C1318" t="n">
         <v>0.172</v>
       </c>
-      <c r="D1318"/>
-      <c r="E1318"/>
+      <c r="D1318" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1318" t="n">
+        <v>0</v>
+      </c>
       <c r="F1318" t="n">
         <v>4.11</v>
       </c>
@@ -56907,8 +57589,12 @@
       <c r="C1319" t="n">
         <v>0.11</v>
       </c>
-      <c r="D1319"/>
-      <c r="E1319"/>
+      <c r="D1319" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1319" t="n">
+        <v>0</v>
+      </c>
       <c r="F1319" t="n">
         <v>4.09</v>
       </c>
@@ -57093,8 +57779,12 @@
       <c r="C1324" t="n">
         <v>0.06</v>
       </c>
-      <c r="D1324"/>
-      <c r="E1324"/>
+      <c r="D1324" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1324" t="n">
+        <v>0</v>
+      </c>
       <c r="F1324" t="n">
         <v>7.38</v>
       </c>
@@ -57127,8 +57817,12 @@
       <c r="C1325" t="n">
         <v>0.086</v>
       </c>
-      <c r="D1325"/>
-      <c r="E1325"/>
+      <c r="D1325" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1325" t="n">
+        <v>0</v>
+      </c>
       <c r="F1325" t="n">
         <v>5.48</v>
       </c>
@@ -57199,8 +57893,12 @@
       <c r="C1327" t="n">
         <v>0.043</v>
       </c>
-      <c r="D1327"/>
-      <c r="E1327"/>
+      <c r="D1327" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1327" t="n">
+        <v>0</v>
+      </c>
       <c r="F1327" t="n">
         <v>6.8</v>
       </c>
@@ -57233,8 +57931,12 @@
       <c r="C1328" t="n">
         <v>0.058</v>
       </c>
-      <c r="D1328"/>
-      <c r="E1328"/>
+      <c r="D1328" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1328" t="n">
+        <v>0</v>
+      </c>
       <c r="F1328" t="n">
         <v>6.56</v>
       </c>
@@ -57267,8 +57969,12 @@
       <c r="C1329" t="n">
         <v>0.046</v>
       </c>
-      <c r="D1329"/>
-      <c r="E1329"/>
+      <c r="D1329" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1329" t="n">
+        <v>0</v>
+      </c>
       <c r="F1329" t="n">
         <v>9.78</v>
       </c>
@@ -57339,8 +58045,12 @@
       <c r="C1331" t="n">
         <v>0.054</v>
       </c>
-      <c r="D1331"/>
-      <c r="E1331"/>
+      <c r="D1331" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1331" t="n">
+        <v>0</v>
+      </c>
       <c r="F1331" t="n">
         <v>7.27</v>
       </c>
@@ -57373,8 +58083,12 @@
       <c r="C1332" t="n">
         <v>0.118</v>
       </c>
-      <c r="D1332"/>
-      <c r="E1332"/>
+      <c r="D1332" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1332" t="n">
+        <v>0</v>
+      </c>
       <c r="F1332" t="n">
         <v>7.44</v>
       </c>
@@ -57407,8 +58121,12 @@
       <c r="C1333" t="n">
         <v>0.118</v>
       </c>
-      <c r="D1333"/>
-      <c r="E1333"/>
+      <c r="D1333" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1333" t="n">
+        <v>0</v>
+      </c>
       <c r="F1333" t="n">
         <v>3.35</v>
       </c>
@@ -57441,8 +58159,12 @@
       <c r="C1334" t="n">
         <v>0.11</v>
       </c>
-      <c r="D1334"/>
-      <c r="E1334"/>
+      <c r="D1334" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1334" t="n">
+        <v>0</v>
+      </c>
       <c r="F1334" t="n">
         <v>1.6</v>
       </c>
@@ -58383,8 +59105,12 @@
       <c r="C1360" t="n">
         <v>0.081</v>
       </c>
-      <c r="D1360"/>
-      <c r="E1360"/>
+      <c r="D1360" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1360" t="n">
+        <v>0</v>
+      </c>
       <c r="F1360" t="n">
         <v>5.45</v>
       </c>
@@ -58707,8 +59433,12 @@
       <c r="C1369" t="n">
         <v>0.17</v>
       </c>
-      <c r="D1369"/>
-      <c r="E1369"/>
+      <c r="D1369" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1369" t="n">
+        <v>0</v>
+      </c>
       <c r="F1369" t="n">
         <v>7.61</v>
       </c>
@@ -59539,8 +60269,12 @@
       <c r="C1391" t="n">
         <v>0.148</v>
       </c>
-      <c r="D1391"/>
-      <c r="E1391"/>
+      <c r="D1391" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1391" t="n">
+        <v>0</v>
+      </c>
       <c r="F1391" t="n">
         <v>8.99</v>
       </c>
@@ -59649,8 +60383,12 @@
       <c r="C1394" t="n">
         <v>0.114</v>
       </c>
-      <c r="D1394"/>
-      <c r="E1394"/>
+      <c r="D1394" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1394" t="n">
+        <v>0</v>
+      </c>
       <c r="F1394" t="n">
         <v>7.55</v>
       </c>
@@ -59949,8 +60687,12 @@
       <c r="C1402" t="n">
         <v>0.13</v>
       </c>
-      <c r="D1402"/>
-      <c r="E1402"/>
+      <c r="D1402" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1402" t="n">
+        <v>0</v>
+      </c>
       <c r="F1402" t="n">
         <v>5.84</v>
       </c>
@@ -60021,8 +60763,12 @@
       <c r="C1404" t="n">
         <v>0.072</v>
       </c>
-      <c r="D1404"/>
-      <c r="E1404"/>
+      <c r="D1404" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1404" t="n">
+        <v>0</v>
+      </c>
       <c r="F1404" t="n">
         <v>7.42</v>
       </c>
@@ -60093,8 +60839,12 @@
       <c r="C1406" t="n">
         <v>0.11</v>
       </c>
-      <c r="D1406"/>
-      <c r="E1406"/>
+      <c r="D1406" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1406" t="n">
+        <v>0</v>
+      </c>
       <c r="F1406" t="n">
         <v>6.63</v>
       </c>
@@ -60393,8 +61143,12 @@
       <c r="C1414" t="n">
         <v>0.139</v>
       </c>
-      <c r="D1414"/>
-      <c r="E1414"/>
+      <c r="D1414" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1414" t="n">
+        <v>0</v>
+      </c>
       <c r="F1414" t="n">
         <v>6.78</v>
       </c>
@@ -60617,8 +61371,12 @@
       <c r="C1420" t="n">
         <v>0.114</v>
       </c>
-      <c r="D1420"/>
-      <c r="E1420"/>
+      <c r="D1420" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1420" t="n">
+        <v>0</v>
+      </c>
       <c r="F1420" t="n">
         <v>8.15</v>
       </c>
@@ -60689,8 +61447,12 @@
       <c r="C1422" t="n">
         <v>0.092</v>
       </c>
-      <c r="D1422"/>
-      <c r="E1422"/>
+      <c r="D1422" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1422" t="n">
+        <v>0</v>
+      </c>
       <c r="F1422" t="n">
         <v>5.99</v>
       </c>
@@ -60875,8 +61637,12 @@
       <c r="C1427" t="n">
         <v>0.113</v>
       </c>
-      <c r="D1427"/>
-      <c r="E1427"/>
+      <c r="D1427" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1427" t="n">
+        <v>0</v>
+      </c>
       <c r="F1427" t="n">
         <v>7.73</v>
       </c>
@@ -60947,8 +61713,12 @@
       <c r="C1429" t="n">
         <v>0.036</v>
       </c>
-      <c r="D1429"/>
-      <c r="E1429"/>
+      <c r="D1429" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1429" t="n">
+        <v>0</v>
+      </c>
       <c r="F1429" t="n">
         <v>8.72</v>
       </c>
@@ -61361,8 +62131,12 @@
       <c r="C1440" t="n">
         <v>0.037</v>
       </c>
-      <c r="D1440"/>
-      <c r="E1440"/>
+      <c r="D1440" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1440" t="n">
+        <v>0</v>
+      </c>
       <c r="F1440" t="n">
         <v>17.26</v>
       </c>
@@ -63219,8 +63993,12 @@
       <c r="C1489" t="n">
         <v>0.081</v>
       </c>
-      <c r="D1489"/>
-      <c r="E1489"/>
+      <c r="D1489" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1489" t="n">
+        <v>0</v>
+      </c>
       <c r="F1489" t="n">
         <v>10.09</v>
       </c>
@@ -63823,8 +64601,12 @@
       <c r="C1505" t="n">
         <v>0.076</v>
       </c>
-      <c r="D1505"/>
-      <c r="E1505"/>
+      <c r="D1505" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1505" t="n">
+        <v>0</v>
+      </c>
       <c r="F1505" t="n">
         <v>11.36</v>
       </c>
@@ -63895,8 +64677,12 @@
       <c r="C1507" t="n">
         <v>0.036</v>
       </c>
-      <c r="D1507"/>
-      <c r="E1507"/>
+      <c r="D1507" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1507" t="n">
+        <v>0</v>
+      </c>
       <c r="F1507" t="n">
         <v>12.89</v>
       </c>
@@ -64309,8 +65095,12 @@
       <c r="C1518" t="n">
         <v>0.027</v>
       </c>
-      <c r="D1518"/>
-      <c r="E1518"/>
+      <c r="D1518" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1518" t="n">
+        <v>0</v>
+      </c>
       <c r="F1518" t="n">
         <v>9.56</v>
       </c>
@@ -64910,7 +65700,9 @@
       <c r="B1534" t="n">
         <v>93.769</v>
       </c>
-      <c r="C1534"/>
+      <c r="C1534" t="n">
+        <v>0</v>
+      </c>
       <c r="D1534" t="n">
         <v>455</v>
       </c>
@@ -65008,7 +65800,9 @@
       <c r="B1537" t="n">
         <v>94.923</v>
       </c>
-      <c r="C1537"/>
+      <c r="C1537" t="n">
+        <v>0</v>
+      </c>
       <c r="D1537" t="n">
         <v>352.8</v>
       </c>
@@ -65386,7 +66180,9 @@
       <c r="B1547" t="n">
         <v>93.157</v>
       </c>
-      <c r="C1547"/>
+      <c r="C1547" t="n">
+        <v>0</v>
+      </c>
       <c r="D1547" t="n">
         <v>775.4</v>
       </c>
@@ -65460,7 +66256,9 @@
       <c r="B1549" t="n">
         <v>95.793</v>
       </c>
-      <c r="C1549"/>
+      <c r="C1549" t="n">
+        <v>0</v>
+      </c>
       <c r="D1549" t="n">
         <v>528.5</v>
       </c>
@@ -67658,7 +68456,9 @@
       <c r="B1608" t="n">
         <v>99.172</v>
       </c>
-      <c r="C1608"/>
+      <c r="C1608" t="n">
+        <v>0</v>
+      </c>
       <c r="D1608" t="n">
         <v>2060.2</v>
       </c>
@@ -67963,8 +68763,12 @@
       <c r="C1616" t="n">
         <v>0.014</v>
       </c>
-      <c r="D1616"/>
-      <c r="E1616"/>
+      <c r="D1616" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1616" t="n">
+        <v>0</v>
+      </c>
       <c r="F1616" t="n">
         <v>5.49</v>
       </c>
@@ -68146,7 +68950,9 @@
       <c r="B1621" t="n">
         <v>101.707</v>
       </c>
-      <c r="C1621"/>
+      <c r="C1621" t="n">
+        <v>0</v>
+      </c>
       <c r="D1621" t="n">
         <v>2878</v>
       </c>
@@ -69954,7 +70760,9 @@
       <c r="B1669" t="n">
         <v>94.93</v>
       </c>
-      <c r="C1669"/>
+      <c r="C1669" t="n">
+        <v>0</v>
+      </c>
       <c r="D1669" t="n">
         <v>66.2</v>
       </c>
@@ -69979,8 +70787,12 @@
       <c r="C1670" t="n">
         <v>0.01</v>
       </c>
-      <c r="D1670"/>
-      <c r="E1670"/>
+      <c r="D1670" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1670" t="n">
+        <v>0</v>
+      </c>
       <c r="F1670" t="n">
         <v>9.05</v>
       </c>
@@ -70089,8 +70901,12 @@
       <c r="C1673" t="n">
         <v>0.054</v>
       </c>
-      <c r="D1673"/>
-      <c r="E1673"/>
+      <c r="D1673" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1673" t="n">
+        <v>0</v>
+      </c>
       <c r="F1673" t="n">
         <v>9.13</v>
       </c>
@@ -70769,8 +71585,12 @@
       <c r="C1691" t="n">
         <v>0.139</v>
       </c>
-      <c r="D1691"/>
-      <c r="E1691"/>
+      <c r="D1691" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1691" t="n">
+        <v>0</v>
+      </c>
       <c r="F1691" t="n">
         <v>7.52</v>
       </c>
@@ -71321,8 +72141,12 @@
       <c r="C1706" t="n">
         <v>0.009</v>
       </c>
-      <c r="D1706"/>
-      <c r="E1706"/>
+      <c r="D1706" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1706" t="n">
+        <v>0</v>
+      </c>
       <c r="F1706" t="n">
         <v>8.57</v>
       </c>
@@ -71656,7 +72480,9 @@
       <c r="B1715" t="n">
         <v>93.558</v>
       </c>
-      <c r="C1715"/>
+      <c r="C1715" t="n">
+        <v>0</v>
+      </c>
       <c r="D1715" t="n">
         <v>24.2</v>
       </c>
@@ -71999,8 +72825,12 @@
       <c r="C1724" t="n">
         <v>0.017</v>
       </c>
-      <c r="D1724"/>
-      <c r="E1724"/>
+      <c r="D1724" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1724" t="n">
+        <v>0</v>
+      </c>
       <c r="F1724" t="n">
         <v>8.27</v>
       </c>
@@ -72831,8 +73661,12 @@
       <c r="C1746" t="n">
         <v>0.05</v>
       </c>
-      <c r="D1746"/>
-      <c r="E1746"/>
+      <c r="D1746" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1746" t="n">
+        <v>0</v>
+      </c>
       <c r="F1746" t="n">
         <v>7.2</v>
       </c>
@@ -73093,8 +73927,12 @@
       <c r="C1753" t="n">
         <v>0.115</v>
       </c>
-      <c r="D1753"/>
-      <c r="E1753"/>
+      <c r="D1753" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1753" t="n">
+        <v>0</v>
+      </c>
       <c r="F1753" t="n">
         <v>7.64</v>
       </c>
@@ -75527,8 +76365,12 @@
       <c r="C1819" t="n">
         <v>0.009</v>
       </c>
-      <c r="D1819"/>
-      <c r="E1819"/>
+      <c r="D1819" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1819" t="n">
+        <v>0</v>
+      </c>
       <c r="F1819"/>
       <c r="G1819"/>
       <c r="H1819"/>
@@ -75965,8 +76807,12 @@
       <c r="C1831" t="n">
         <v>0.003</v>
       </c>
-      <c r="D1831"/>
-      <c r="E1831"/>
+      <c r="D1831" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1831" t="n">
+        <v>0</v>
+      </c>
       <c r="F1831" t="n">
         <v>7.58</v>
       </c>
@@ -77312,7 +78158,9 @@
       <c r="B1867" t="n">
         <v>95.006</v>
       </c>
-      <c r="C1867"/>
+      <c r="C1867" t="n">
+        <v>0</v>
+      </c>
       <c r="D1867" t="n">
         <v>510.6</v>
       </c>
@@ -79990,7 +80838,9 @@
       <c r="B1939" t="n">
         <v>99.351</v>
       </c>
-      <c r="C1939"/>
+      <c r="C1939" t="n">
+        <v>0</v>
+      </c>
       <c r="D1939" t="n">
         <v>2997.2</v>
       </c>
@@ -80112,7 +80962,9 @@
       <c r="B1943" t="n">
         <v>99.458</v>
       </c>
-      <c r="C1943"/>
+      <c r="C1943" t="n">
+        <v>0</v>
+      </c>
       <c r="D1943" t="n">
         <v>2381.2</v>
       </c>
@@ -80721,8 +81573,12 @@
       <c r="C1959" t="n">
         <v>0.012</v>
       </c>
-      <c r="D1959"/>
-      <c r="E1959"/>
+      <c r="D1959" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1959" t="n">
+        <v>0</v>
+      </c>
       <c r="F1959" t="n">
         <v>4.85</v>
       </c>
@@ -83208,7 +84064,9 @@
       <c r="B2025" t="n">
         <v>92.248</v>
       </c>
-      <c r="C2025"/>
+      <c r="C2025" t="n">
+        <v>0</v>
+      </c>
       <c r="D2025" t="n">
         <v>856.4</v>
       </c>
@@ -83703,8 +84561,12 @@
       <c r="C2038" t="n">
         <v>0.008</v>
       </c>
-      <c r="D2038"/>
-      <c r="E2038"/>
+      <c r="D2038" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2038" t="n">
+        <v>0</v>
+      </c>
       <c r="F2038" t="n">
         <v>8.32</v>
       </c>
@@ -83775,8 +84637,12 @@
       <c r="C2040" t="n">
         <v>0.027</v>
       </c>
-      <c r="D2040"/>
-      <c r="E2040"/>
+      <c r="D2040" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2040" t="n">
+        <v>0</v>
+      </c>
       <c r="F2040" t="n">
         <v>9.18</v>
       </c>
@@ -83809,8 +84675,12 @@
       <c r="C2041" t="n">
         <v>0.008</v>
       </c>
-      <c r="D2041"/>
-      <c r="E2041"/>
+      <c r="D2041" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2041" t="n">
+        <v>0</v>
+      </c>
       <c r="F2041" t="n">
         <v>5.72</v>
       </c>
@@ -84527,8 +85397,12 @@
       <c r="C2060" t="n">
         <v>0.067</v>
       </c>
-      <c r="D2060"/>
-      <c r="E2060"/>
+      <c r="D2060" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2060" t="n">
+        <v>0</v>
+      </c>
       <c r="F2060" t="n">
         <v>19.65</v>
       </c>
@@ -84675,8 +85549,12 @@
       <c r="C2064" t="n">
         <v>0.074</v>
       </c>
-      <c r="D2064"/>
-      <c r="E2064"/>
+      <c r="D2064" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2064" t="n">
+        <v>0</v>
+      </c>
       <c r="F2064" t="n">
         <v>9.45</v>
       </c>
@@ -85051,8 +85929,12 @@
       <c r="C2074" t="n">
         <v>0.036</v>
       </c>
-      <c r="D2074"/>
-      <c r="E2074"/>
+      <c r="D2074" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2074" t="n">
+        <v>0</v>
+      </c>
       <c r="F2074" t="n">
         <v>8.21</v>
       </c>
@@ -85845,8 +86727,12 @@
       <c r="C2095" t="n">
         <v>0.093</v>
       </c>
-      <c r="D2095"/>
-      <c r="E2095"/>
+      <c r="D2095" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2095" t="n">
+        <v>0</v>
+      </c>
       <c r="F2095" t="n">
         <v>6.36</v>
       </c>
@@ -86525,8 +87411,12 @@
       <c r="C2113" t="n">
         <v>0.084</v>
       </c>
-      <c r="D2113"/>
-      <c r="E2113"/>
+      <c r="D2113" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2113" t="n">
+        <v>0</v>
+      </c>
       <c r="F2113" t="n">
         <v>7.52</v>
       </c>
@@ -87267,8 +88157,12 @@
       <c r="C2133" t="n">
         <v>0.064</v>
       </c>
-      <c r="D2133"/>
-      <c r="E2133"/>
+      <c r="D2133" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2133" t="n">
+        <v>0</v>
+      </c>
       <c r="F2133" t="n">
         <v>8.77</v>
       </c>
@@ -87857,8 +88751,12 @@
       <c r="C2149" t="n">
         <v>0.018</v>
       </c>
-      <c r="D2149"/>
-      <c r="E2149"/>
+      <c r="D2149" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2149" t="n">
+        <v>0</v>
+      </c>
       <c r="F2149" t="n">
         <v>12.19</v>
       </c>
@@ -90727,8 +91625,12 @@
       <c r="C2225" t="n">
         <v>0.031</v>
       </c>
-      <c r="D2225"/>
-      <c r="E2225"/>
+      <c r="D2225" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2225" t="n">
+        <v>0</v>
+      </c>
       <c r="F2225" t="n">
         <v>5.89</v>
       </c>
@@ -91255,8 +92157,12 @@
       <c r="C2239" t="n">
         <v>0.048</v>
       </c>
-      <c r="D2239"/>
-      <c r="E2239"/>
+      <c r="D2239" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2239" t="n">
+        <v>0</v>
+      </c>
       <c r="F2239" t="n">
         <v>10.09</v>
       </c>
@@ -91479,8 +92385,12 @@
       <c r="C2245" t="n">
         <v>0.022</v>
       </c>
-      <c r="D2245"/>
-      <c r="E2245"/>
+      <c r="D2245" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2245" t="n">
+        <v>0</v>
+      </c>
       <c r="F2245" t="n">
         <v>6.25</v>
       </c>
@@ -92156,7 +93066,9 @@
       <c r="B2263" t="n">
         <v>94.778</v>
       </c>
-      <c r="C2263"/>
+      <c r="C2263" t="n">
+        <v>0</v>
+      </c>
       <c r="D2263" t="n">
         <v>681.8</v>
       </c>
@@ -92195,8 +93107,12 @@
       <c r="C2264" t="n">
         <v>0.006</v>
       </c>
-      <c r="D2264"/>
-      <c r="E2264"/>
+      <c r="D2264" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2264" t="n">
+        <v>0</v>
+      </c>
       <c r="F2264" t="n">
         <v>7.46</v>
       </c>
@@ -92671,8 +93587,12 @@
       <c r="C2277" t="n">
         <v>0.036</v>
       </c>
-      <c r="D2277"/>
-      <c r="E2277"/>
+      <c r="D2277" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2277" t="n">
+        <v>0</v>
+      </c>
       <c r="F2277" t="n">
         <v>6.58</v>
       </c>
@@ -92819,8 +93739,12 @@
       <c r="C2281" t="n">
         <v>0.038</v>
       </c>
-      <c r="D2281"/>
-      <c r="E2281"/>
+      <c r="D2281" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2281" t="n">
+        <v>0</v>
+      </c>
       <c r="F2281" t="n">
         <v>7.1</v>
       </c>
@@ -93979,8 +94903,12 @@
       <c r="C2312" t="n">
         <v>0.008</v>
       </c>
-      <c r="D2312"/>
-      <c r="E2312"/>
+      <c r="D2312" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2312" t="n">
+        <v>0</v>
+      </c>
       <c r="F2312" t="n">
         <v>6.5</v>
       </c>
@@ -94355,8 +95283,12 @@
       <c r="C2322" t="n">
         <v>0.048</v>
       </c>
-      <c r="D2322"/>
-      <c r="E2322"/>
+      <c r="D2322" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2322" t="n">
+        <v>0</v>
+      </c>
       <c r="F2322" t="n">
         <v>5.99</v>
       </c>
@@ -94541,8 +95473,12 @@
       <c r="C2327" t="n">
         <v>0.047</v>
       </c>
-      <c r="D2327"/>
-      <c r="E2327"/>
+      <c r="D2327" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2327" t="n">
+        <v>0</v>
+      </c>
       <c r="F2327" t="n">
         <v>6.27</v>
       </c>
@@ -94765,8 +95701,12 @@
       <c r="C2333" t="n">
         <v>0.036</v>
       </c>
-      <c r="D2333"/>
-      <c r="E2333"/>
+      <c r="D2333" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2333" t="n">
+        <v>0</v>
+      </c>
       <c r="F2333" t="n">
         <v>6.7</v>
       </c>
@@ -94913,8 +95853,12 @@
       <c r="C2337" t="n">
         <v>0.042</v>
       </c>
-      <c r="D2337"/>
-      <c r="E2337"/>
+      <c r="D2337" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2337" t="n">
+        <v>0</v>
+      </c>
       <c r="F2337" t="n">
         <v>7.37</v>
       </c>
@@ -95973,8 +96917,12 @@
       <c r="C2365" t="n">
         <v>0.023</v>
       </c>
-      <c r="D2365"/>
-      <c r="E2365"/>
+      <c r="D2365" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2365" t="n">
+        <v>0</v>
+      </c>
       <c r="F2365" t="n">
         <v>7.65</v>
       </c>
@@ -96007,8 +96955,12 @@
       <c r="C2366" t="n">
         <v>0.144</v>
       </c>
-      <c r="D2366"/>
-      <c r="E2366"/>
+      <c r="D2366" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2366" t="n">
+        <v>0</v>
+      </c>
       <c r="F2366" t="n">
         <v>7.34</v>
       </c>
@@ -96649,8 +97601,12 @@
       <c r="C2383" t="n">
         <v>0.04</v>
       </c>
-      <c r="D2383"/>
-      <c r="E2383"/>
+      <c r="D2383" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2383" t="n">
+        <v>0</v>
+      </c>
       <c r="F2383" t="n">
         <v>14.78</v>
       </c>
@@ -96797,8 +97753,12 @@
       <c r="C2387" t="n">
         <v>0.057</v>
       </c>
-      <c r="D2387"/>
-      <c r="E2387"/>
+      <c r="D2387" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2387" t="n">
+        <v>0</v>
+      </c>
       <c r="F2387" t="n">
         <v>9.2</v>
       </c>
@@ -97591,8 +98551,12 @@
       <c r="C2408" t="n">
         <v>0.09</v>
       </c>
-      <c r="D2408"/>
-      <c r="E2408"/>
+      <c r="D2408" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2408" t="n">
+        <v>0</v>
+      </c>
       <c r="F2408" t="n">
         <v>12.68</v>
       </c>
@@ -97663,8 +98627,12 @@
       <c r="C2410" t="n">
         <v>0.049</v>
       </c>
-      <c r="D2410"/>
-      <c r="E2410"/>
+      <c r="D2410" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2410" t="n">
+        <v>0</v>
+      </c>
       <c r="F2410" t="n">
         <v>15.42</v>
       </c>
@@ -98153,8 +99121,12 @@
       <c r="C2423" t="n">
         <v>0.036</v>
       </c>
-      <c r="D2423"/>
-      <c r="E2423"/>
+      <c r="D2423" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2423" t="n">
+        <v>0</v>
+      </c>
       <c r="F2423" t="n">
         <v>10.61</v>
       </c>
@@ -99213,8 +100185,12 @@
       <c r="C2451" t="n">
         <v>0.058</v>
       </c>
-      <c r="D2451"/>
-      <c r="E2451"/>
+      <c r="D2451" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2451" t="n">
+        <v>0</v>
+      </c>
       <c r="F2451" t="n">
         <v>8.36</v>
       </c>
@@ -99599,8 +100575,12 @@
       <c r="C2462" t="n">
         <v>0.07</v>
       </c>
-      <c r="D2462"/>
-      <c r="E2462"/>
+      <c r="D2462" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2462" t="n">
+        <v>0</v>
+      </c>
       <c r="F2462" t="n">
         <v>6.86</v>
       </c>
@@ -100835,8 +101815,12 @@
       <c r="C2495" t="n">
         <v>0.027</v>
       </c>
-      <c r="D2495"/>
-      <c r="E2495"/>
+      <c r="D2495" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2495" t="n">
+        <v>0</v>
+      </c>
       <c r="F2495" t="n">
         <v>5.9</v>
       </c>
@@ -100907,8 +101891,12 @@
       <c r="C2497" t="n">
         <v>0.02</v>
       </c>
-      <c r="D2497"/>
-      <c r="E2497"/>
+      <c r="D2497" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2497" t="n">
+        <v>0</v>
+      </c>
       <c r="F2497" t="n">
         <v>6.95</v>
       </c>
@@ -101283,8 +102271,12 @@
       <c r="C2507" t="n">
         <v>0.017</v>
       </c>
-      <c r="D2507"/>
-      <c r="E2507"/>
+      <c r="D2507" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2507" t="n">
+        <v>0</v>
+      </c>
       <c r="F2507" t="n">
         <v>8.12</v>
       </c>
@@ -101355,8 +102347,12 @@
       <c r="C2509" t="n">
         <v>0.047</v>
       </c>
-      <c r="D2509"/>
-      <c r="E2509"/>
+      <c r="D2509" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2509" t="n">
+        <v>0</v>
+      </c>
       <c r="F2509" t="n">
         <v>7.59</v>
       </c>
@@ -101427,8 +102423,12 @@
       <c r="C2511" t="n">
         <v>0.075</v>
       </c>
-      <c r="D2511"/>
-      <c r="E2511"/>
+      <c r="D2511" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2511" t="n">
+        <v>0</v>
+      </c>
       <c r="F2511" t="n">
         <v>5.45</v>
       </c>
@@ -101461,8 +102461,12 @@
       <c r="C2512" t="n">
         <v>0.069</v>
       </c>
-      <c r="D2512"/>
-      <c r="E2512"/>
+      <c r="D2512" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2512" t="n">
+        <v>0</v>
+      </c>
       <c r="F2512" t="n">
         <v>6.13</v>
       </c>
@@ -101609,8 +102613,12 @@
       <c r="C2516" t="n">
         <v>0.021</v>
       </c>
-      <c r="D2516"/>
-      <c r="E2516"/>
+      <c r="D2516" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2516" t="n">
+        <v>0</v>
+      </c>
       <c r="F2516" t="n">
         <v>8.67</v>
       </c>
@@ -101719,8 +102727,12 @@
       <c r="C2519" t="n">
         <v>0.03</v>
       </c>
-      <c r="D2519"/>
-      <c r="E2519"/>
+      <c r="D2519" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2519" t="n">
+        <v>0</v>
+      </c>
       <c r="F2519" t="n">
         <v>9.55</v>
       </c>
@@ -101753,8 +102765,12 @@
       <c r="C2520" t="n">
         <v>0.059</v>
       </c>
-      <c r="D2520"/>
-      <c r="E2520"/>
+      <c r="D2520" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2520" t="n">
+        <v>0</v>
+      </c>
       <c r="F2520" t="n">
         <v>5.15</v>
       </c>
@@ -101939,8 +102955,12 @@
       <c r="C2525" t="n">
         <v>0.021</v>
       </c>
-      <c r="D2525"/>
-      <c r="E2525"/>
+      <c r="D2525" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2525" t="n">
+        <v>0</v>
+      </c>
       <c r="F2525" t="n">
         <v>6.86</v>
       </c>
@@ -102011,8 +103031,12 @@
       <c r="C2527" t="n">
         <v>0.049</v>
       </c>
-      <c r="D2527"/>
-      <c r="E2527"/>
+      <c r="D2527" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2527" t="n">
+        <v>0</v>
+      </c>
       <c r="F2527" t="n">
         <v>6.31</v>
       </c>
@@ -102045,8 +103069,12 @@
       <c r="C2528" t="n">
         <v>0.047</v>
       </c>
-      <c r="D2528"/>
-      <c r="E2528"/>
+      <c r="D2528" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2528" t="n">
+        <v>0</v>
+      </c>
       <c r="F2528" t="n">
         <v>5.61</v>
       </c>
@@ -102079,8 +103107,12 @@
       <c r="C2529" t="n">
         <v>0.057</v>
       </c>
-      <c r="D2529"/>
-      <c r="E2529"/>
+      <c r="D2529" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2529" t="n">
+        <v>0</v>
+      </c>
       <c r="F2529" t="n">
         <v>6.54</v>
       </c>
@@ -102113,8 +103145,12 @@
       <c r="C2530" t="n">
         <v>0</v>
       </c>
-      <c r="D2530"/>
-      <c r="E2530"/>
+      <c r="D2530" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2530" t="n">
+        <v>0</v>
+      </c>
       <c r="F2530" t="n">
         <v>5.86</v>
       </c>
@@ -102223,8 +103259,12 @@
       <c r="C2533" t="n">
         <v>0.024</v>
       </c>
-      <c r="D2533"/>
-      <c r="E2533"/>
+      <c r="D2533" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2533" t="n">
+        <v>0</v>
+      </c>
       <c r="F2533" t="n">
         <v>6.92</v>
       </c>
@@ -102295,8 +103335,12 @@
       <c r="C2535" t="n">
         <v>0.027</v>
       </c>
-      <c r="D2535"/>
-      <c r="E2535"/>
+      <c r="D2535" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2535" t="n">
+        <v>0</v>
+      </c>
       <c r="F2535" t="n">
         <v>7.19</v>
       </c>
@@ -102633,8 +103677,12 @@
       <c r="C2544" t="n">
         <v>0.056</v>
       </c>
-      <c r="D2544"/>
-      <c r="E2544"/>
+      <c r="D2544" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2544" t="n">
+        <v>0</v>
+      </c>
       <c r="F2544" t="n">
         <v>7.26</v>
       </c>
@@ -102667,8 +103715,12 @@
       <c r="C2545" t="n">
         <v>0.038</v>
       </c>
-      <c r="D2545"/>
-      <c r="E2545"/>
+      <c r="D2545" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2545" t="n">
+        <v>0</v>
+      </c>
       <c r="F2545" t="n">
         <v>7.74</v>
       </c>
@@ -102701,8 +103753,12 @@
       <c r="C2546" t="n">
         <v>0.018</v>
       </c>
-      <c r="D2546"/>
-      <c r="E2546"/>
+      <c r="D2546" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2546" t="n">
+        <v>0</v>
+      </c>
       <c r="F2546" t="n">
         <v>8.26</v>
       </c>
@@ -102963,8 +104019,12 @@
       <c r="C2553" t="n">
         <v>0.049</v>
       </c>
-      <c r="D2553"/>
-      <c r="E2553"/>
+      <c r="D2553" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2553" t="n">
+        <v>0</v>
+      </c>
       <c r="F2553" t="n">
         <v>6.41</v>
       </c>
@@ -103149,8 +104209,12 @@
       <c r="C2558" t="n">
         <v>0.046</v>
       </c>
-      <c r="D2558"/>
-      <c r="E2558"/>
+      <c r="D2558" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2558" t="n">
+        <v>0</v>
+      </c>
       <c r="F2558" t="n">
         <v>8.57</v>
       </c>
@@ -103221,8 +104285,12 @@
       <c r="C2560" t="n">
         <v>0.007</v>
       </c>
-      <c r="D2560"/>
-      <c r="E2560"/>
+      <c r="D2560" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2560" t="n">
+        <v>0</v>
+      </c>
       <c r="F2560" t="n">
         <v>8.16</v>
       </c>
@@ -103255,8 +104323,12 @@
       <c r="C2561" t="n">
         <v>0.025</v>
       </c>
-      <c r="D2561"/>
-      <c r="E2561"/>
+      <c r="D2561" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2561" t="n">
+        <v>0</v>
+      </c>
       <c r="F2561" t="n">
         <v>4.56</v>
       </c>

</xml_diff>